<commit_message>
Prewash- en transform logs naar Excel
</commit_message>
<xml_diff>
--- a/xslweb-jdk8-webservices-docker/home/webapps/excelreport/static/excel/excelreport.xlsx
+++ b/xslweb-jdk8-webservices-docker/home/webapps/excelreport/static/excel/excelreport.xlsx
@@ -11,34 +11,39 @@
     <sheet name="01-Overview" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="02-Unpack" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="03-Virusscan" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="04-Invalid filenames" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="05-Metadata" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="06-Sidecar" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="07-Droid" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="08-Greenlist" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="09-Encoding" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="04-Voorbewerking" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="05-Invalid filenames" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="06-Metadata" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="07-Sidecar" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="08-Droid" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="09-Greenlist" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="10-Encoding" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="11-ToPX2XIP" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Blad2" sheetId="12" state="hidden" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'01-Overview'!$A$1:$L$1</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'02-Unpack'!$A$1</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'03-Virusscan'!$A$1:$C$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'04-Invalid filenames'!$B$1:$D$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'05-Metadata'!$E$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'06-Sidecar'!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">'07-Droid'!$A$1:$R$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">'08-Greenlist'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">'09-Encoding'!$A$1:$C$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'04-Voorbewerking'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'05-Invalid filenames'!$B$1:$D$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'06-Metadata'!$E$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">'07-Sidecar'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">'08-Droid'!$A$1:$R$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">'09-Greenlist'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'10-Encoding'!$A$1:$C$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">'11-ToPX2XIP'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="ExternalData_1" vbProcedure="false">'01-Overview'!$A$1:$B$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="ExternalData_1" vbProcedure="false">'02-Unpack'!$A$1:$A$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'02-Unpack'!$A$1:$A$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">'02-Unpack'!$A$1:$A$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="ExternalData_1" vbProcedure="false">'03-Virusscan'!$A$1:$A$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="ExternalData_1" vbProcedure="false">'04-Invalid filenames'!$A$1:$A$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="ExternalData_1" vbProcedure="false">'05-Metadata'!$A$1:$D$1961</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'05-Metadata'!$E$1:$E$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="ExternalData_2" vbProcedure="false">'06-Sidecar'!$A$1:$C$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="ExternalData_3" vbProcedure="false">'07-Droid'!$A$1:$R$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="ExternalData_1" vbProcedure="false">'08-Greenlist'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="ExternalData_1" vbProcedure="false">'09-Encoding'!$A$1:$C$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="ExternalData_1" vbProcedure="false">'05-Invalid filenames'!$A$1:$A$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="ExternalData_1" vbProcedure="false">'06-Metadata'!$A$1:$D$1961</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0" vbProcedure="false">'06-Metadata'!$E$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="ExternalData_2" vbProcedure="false">'07-Sidecar'!$A$1:$C$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="ExternalData_3" vbProcedure="false">'08-Droid'!$A$1:$R$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="ExternalData_1" vbProcedure="false">'09-Greenlist'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="ExternalData_1" vbProcedure="false">'10-Encoding'!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -50,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t xml:space="preserve">JSON filename</t>
   </si>
@@ -100,6 +105,15 @@
     <t xml:space="preserve">Filename</t>
   </si>
   <si>
+    <t xml:space="preserve">Is washed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RequestUri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MetadataFilename</t>
+  </si>
+  <si>
     <t xml:space="preserve">Invalid characters</t>
   </si>
   <si>
@@ -197,6 +211,9 @@
   </si>
   <si>
     <t xml:space="preserve">UTF-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is transformed</t>
   </si>
 </sst>
 </file>
@@ -322,6 +339,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
@@ -453,6 +478,123 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="182.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="70.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="4" style="2" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="66.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="80.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -497,7 +639,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -534,6 +676,58 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="81.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -556,10 +750,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>15</v>
@@ -584,7 +778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -608,19 +802,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -639,7 +833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -647,7 +841,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -662,10 +856,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>15</v>
@@ -687,7 +881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -724,58 +918,58 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -791,7 +985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -817,25 +1011,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -849,49 +1043,4 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C1048576"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="182.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="70.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="4" style="2" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="9.14"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <autoFilter ref="A1:C1"/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>